<commit_message>
Correção para não retirar os "( )"
</commit_message>
<xml_diff>
--- a/planilha_limpa_.xlsx
+++ b/planilha_limpa_.xlsx
@@ -567,22 +567,22 @@
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Alessandra Meireles da Silva Lourenco</t>
+          <t>ALESSANDRA MEIRELES DA SILVA LOURENCO</t>
         </is>
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>fono lar</t>
+          <t>FONO LAR</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
         <is>
-          <t>cooperado</t>
+          <t>COOPERADO</t>
         </is>
       </c>
       <c r="D2" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -604,7 +604,7 @@
       </c>
       <c r="D3" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -626,14 +626,14 @@
       </c>
       <c r="D4" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1">
       <c r="A5" s="12" t="inlineStr">
         <is>
-          <t>Ana Luisa Rodrigues Vasconcellos</t>
+          <t>ANA LUISA RODRIGUES VASCONCELLOS</t>
         </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
@@ -648,14 +648,14 @@
       </c>
       <c r="D5" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
       <c r="A6" s="12" t="inlineStr">
         <is>
-          <t>Ana Maria da Costa Gomes</t>
+          <t>ANA MARIA DA COSTA GOMES</t>
         </is>
       </c>
       <c r="B6" s="13" t="inlineStr">
@@ -670,7 +670,7 @@
       </c>
       <c r="D6" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -692,7 +692,7 @@
       </c>
       <c r="D7" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -714,7 +714,7 @@
       </c>
       <c r="D8" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -736,7 +736,7 @@
       </c>
       <c r="D9" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -758,7 +758,7 @@
       </c>
       <c r="D10" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -780,14 +780,14 @@
       </c>
       <c r="D11" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="12" ht="18.75" customHeight="1">
       <c r="A12" s="12" t="inlineStr">
         <is>
-          <t>Aretuza Cristina Santos De Azevedo</t>
+          <t>ARETUZA CRISTINA SANTOS DE AZEVEDO</t>
         </is>
       </c>
       <c r="B12" s="13" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="D12" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -824,7 +824,7 @@
       </c>
       <c r="D13" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="D14" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -868,14 +868,14 @@
       </c>
       <c r="D15" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="16" ht="18.75" customHeight="1">
       <c r="A16" s="12" t="inlineStr">
         <is>
-          <t>Catia Silva Gomes Bitencourt</t>
+          <t>CATIA SILVA GOMES BITENCOURT</t>
         </is>
       </c>
       <c r="B16" s="13" t="inlineStr">
@@ -890,14 +890,14 @@
       </c>
       <c r="D16" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="17" ht="18.75" customHeight="1">
       <c r="A17" s="12" t="inlineStr">
         <is>
-          <t>Christiane Bonoto Baptista</t>
+          <t>CHRISTIANE BONOTO BAPTISTA</t>
         </is>
       </c>
       <c r="B17" s="13" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="D17" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -934,14 +934,14 @@
       </c>
       <c r="D18" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="19" ht="18.75" customHeight="1">
       <c r="A19" s="12" t="inlineStr">
         <is>
-          <t>Christina Ribeiro Campos</t>
+          <t>CHRISTINA RIBEIRO CAMPOS</t>
         </is>
       </c>
       <c r="B19" s="13" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="D19" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -978,7 +978,7 @@
       </c>
       <c r="D20" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="D21" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1022,14 +1022,14 @@
       </c>
       <c r="D22" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="23" ht="18.75" customHeight="1">
       <c r="A23" s="12" t="inlineStr">
         <is>
-          <t>Deise Luci Serapiao Reis</t>
+          <t>DEISE LUCI SERAPIAO REIS</t>
         </is>
       </c>
       <c r="B23" s="13" t="inlineStr">
@@ -1044,14 +1044,14 @@
       </c>
       <c r="D23" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="24" ht="18.75" customHeight="1">
       <c r="A24" s="12" t="inlineStr">
         <is>
-          <t>Denise Hargreaves Noguera</t>
+          <t>DENISE HARGREAVES NOGUERA</t>
         </is>
       </c>
       <c r="B24" s="13" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="D24" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="D25" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="D26" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="D27" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="D28" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="D29" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="D30" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1220,14 +1220,14 @@
       </c>
       <c r="D31" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="32" ht="18.75" customHeight="1">
       <c r="A32" s="12" t="inlineStr">
         <is>
-          <t>Glauci Pinto de Moraes</t>
+          <t>GLAUCI PINTO DE MORAES</t>
         </is>
       </c>
       <c r="B32" s="13" t="inlineStr">
@@ -1242,14 +1242,14 @@
       </c>
       <c r="D32" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="33" ht="18.75" customHeight="1">
       <c r="A33" s="12" t="inlineStr">
         <is>
-          <t>Hilda Barreto Pinto</t>
+          <t>HILDA BARRETO PINTO</t>
         </is>
       </c>
       <c r="B33" s="13" t="inlineStr">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="D33" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1286,14 +1286,14 @@
       </c>
       <c r="D34" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="35" ht="18.75" customHeight="1">
       <c r="A35" s="12" t="inlineStr">
         <is>
-          <t>Ismeralda Silva de Paula</t>
+          <t>ISMERALDA SILVA DE PAULA</t>
         </is>
       </c>
       <c r="B35" s="13" t="inlineStr">
@@ -1308,14 +1308,14 @@
       </c>
       <c r="D35" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="36" ht="18.75" customHeight="1">
       <c r="A36" s="12" t="inlineStr">
         <is>
-          <t>Ivana Forca da Rocha Vaz</t>
+          <t>IVANA FORCA DA ROCHA VAZ</t>
         </is>
       </c>
       <c r="B36" s="13" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="D36" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1352,14 +1352,14 @@
       </c>
       <c r="D37" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="38" ht="18.75" customHeight="1">
       <c r="A38" s="12" t="inlineStr">
         <is>
-          <t>Jane Cruz dos Santos</t>
+          <t>JANE CRUZ DOS SANTOS</t>
         </is>
       </c>
       <c r="B38" s="13" t="inlineStr">
@@ -1374,14 +1374,14 @@
       </c>
       <c r="D38" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="39" ht="12" customHeight="1">
       <c r="A39" s="12" t="inlineStr">
         <is>
-          <t>Jaqueline Fontoura da Cunha</t>
+          <t>JAQUELINE FONTOURA DA CUNHA</t>
         </is>
       </c>
       <c r="B39" s="13" t="inlineStr">
@@ -1396,14 +1396,14 @@
       </c>
       <c r="D39" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="40" ht="12" customHeight="1">
       <c r="A40" s="12" t="inlineStr">
         <is>
-          <t>Jessica Caroline Lopes da Cunha Frazao</t>
+          <t>JESSICA CAROLINE LOPES DA CUNHA FRAZAO</t>
         </is>
       </c>
       <c r="B40" s="13" t="inlineStr">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="D40" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="D41" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="D42" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="D43" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="D44" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="D45" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="D46" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="D47" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1594,14 +1594,14 @@
       </c>
       <c r="D48" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="49" ht="12" customHeight="1">
       <c r="A49" s="12" t="inlineStr">
         <is>
-          <t>Luciana de Carvalho Conceicao</t>
+          <t>LUCIANA DE CARVALHO CONCEICAO</t>
         </is>
       </c>
       <c r="B49" s="13" t="inlineStr">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="D49" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="D50" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="D51" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="D52" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="D53" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1726,14 +1726,14 @@
       </c>
       <c r="D54" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="55" ht="12" customHeight="1">
       <c r="A55" s="12" t="inlineStr">
         <is>
-          <t>Maria Luiza Fontanella</t>
+          <t>MARIA LUIZA FONTANELLA</t>
         </is>
       </c>
       <c r="B55" s="13" t="inlineStr">
@@ -1748,14 +1748,14 @@
       </c>
       <c r="D55" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="56" ht="12" customHeight="1">
       <c r="A56" s="12" t="inlineStr">
         <is>
-          <t>Mariana Goncalves Vieira</t>
+          <t>MARIANA GONCALVES VIEIRA</t>
         </is>
       </c>
       <c r="B56" s="13" t="inlineStr">
@@ -1770,7 +1770,7 @@
       </c>
       <c r="D56" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D57" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="D58" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1836,14 +1836,14 @@
       </c>
       <c r="D59" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="60" ht="12" customHeight="1">
       <c r="A60" s="12" t="inlineStr">
         <is>
-          <t>Natasha Boulhosa da Silva</t>
+          <t>NATASHA BOULHOSA DA SILVA</t>
         </is>
       </c>
       <c r="B60" s="13" t="inlineStr">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="D60" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1880,14 +1880,14 @@
       </c>
       <c r="D61" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="62" ht="12" customHeight="1">
       <c r="A62" s="12" t="inlineStr">
         <is>
-          <t>Patricia Abreu de Freitas</t>
+          <t>PATRICIA ABREU DE FREITAS</t>
         </is>
       </c>
       <c r="B62" s="13" t="inlineStr">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="D62" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="D63" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="D64" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1968,7 +1968,7 @@
       </c>
       <c r="D65" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="D66" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2012,14 +2012,14 @@
       </c>
       <c r="D67" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="68" ht="12" customHeight="1">
       <c r="A68" s="12" t="inlineStr">
         <is>
-          <t>Rafael Ramos De Pontes</t>
+          <t>RAFAEL RAMOS DE PONTES</t>
         </is>
       </c>
       <c r="B68" s="13" t="inlineStr">
@@ -2034,14 +2034,14 @@
       </c>
       <c r="D68" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="69" ht="12" customHeight="1">
       <c r="A69" s="12" t="inlineStr">
         <is>
-          <t>Rafaella Santos da Silva</t>
+          <t>RAFAELLA SANTOS DA SILVA</t>
         </is>
       </c>
       <c r="B69" s="13" t="inlineStr">
@@ -2056,14 +2056,14 @@
       </c>
       <c r="D69" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="70" ht="12" customHeight="1">
       <c r="A70" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Raphaelli Mourant Goncalves </t>
+          <t xml:space="preserve">RAPHAELLI MOURANT GONCALVES </t>
         </is>
       </c>
       <c r="B70" s="13" t="inlineStr">
@@ -2078,14 +2078,14 @@
       </c>
       <c r="D70" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="71" ht="12" customHeight="1">
       <c r="A71" s="12" t="inlineStr">
         <is>
-          <t>Regina Auxiliadora Muniz Teixeira</t>
+          <t>REGINA AUXILIADORA MUNIZ TEIXEIRA</t>
         </is>
       </c>
       <c r="B71" s="13" t="inlineStr">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="D71" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="D72" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2144,14 +2144,14 @@
       </c>
       <c r="D73" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="74" ht="12" customHeight="1">
       <c r="A74" s="12" t="inlineStr">
         <is>
-          <t>Renata Nogueira de Aguiar</t>
+          <t>RENATA NOGUEIRA DE AGUIAR</t>
         </is>
       </c>
       <c r="B74" s="13" t="inlineStr">
@@ -2166,14 +2166,14 @@
       </c>
       <c r="D74" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="75" ht="12" customHeight="1">
       <c r="A75" s="12" t="inlineStr">
         <is>
-          <t>Rita De Cassia Carvalhal Moreira Dos Santos</t>
+          <t>RITA DE CASSIA CARVALHAL MOREIRA DOS SANTOS</t>
         </is>
       </c>
       <c r="B75" s="13" t="inlineStr">
@@ -2188,14 +2188,14 @@
       </c>
       <c r="D75" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="76" ht="12" customHeight="1">
       <c r="A76" s="12" t="inlineStr">
         <is>
-          <t>Rosa Maria Costa Salinas</t>
+          <t>ROSA MARIA COSTA SALINAS</t>
         </is>
       </c>
       <c r="B76" s="13" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="D76" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="D77" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="D78" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="D79" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2298,14 +2298,14 @@
       </c>
       <c r="D80" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="81" ht="12" customHeight="1">
       <c r="A81" s="12" t="inlineStr">
         <is>
-          <t>Silvia Suemi Horigome</t>
+          <t>SILVIA SUEMI HORIGOME</t>
         </is>
       </c>
       <c r="B81" s="13" t="inlineStr">
@@ -2320,14 +2320,14 @@
       </c>
       <c r="D81" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="82" ht="12" customHeight="1">
       <c r="A82" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sonia Maria Silva </t>
+          <t xml:space="preserve">SONIA MARIA SILVA </t>
         </is>
       </c>
       <c r="B82" s="13" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="D82" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="D83" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2386,7 +2386,7 @@
       </c>
       <c r="D84" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="D85" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
@@ -2430,14 +2430,14 @@
       </c>
       <c r="D86" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="87" ht="12" customHeight="1">
       <c r="A87" s="12" t="inlineStr">
         <is>
-          <t>Veronica dos Santos Sousa</t>
+          <t>VERONICA DOS SANTOS SOUSA</t>
         </is>
       </c>
       <c r="B87" s="13" t="inlineStr">
@@ -2452,14 +2452,14 @@
       </c>
       <c r="D87" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>
     <row r="88" ht="12" customHeight="1">
       <c r="A88" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yanna Bravim Paulino </t>
+          <t xml:space="preserve">YANNA BRAVIM PAULINO </t>
         </is>
       </c>
       <c r="B88" s="13" t="inlineStr">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="D88" s="12" t="inlineStr">
         <is>
-          <t>Fonoaudiologo a</t>
+          <t>FONOAUDIOLOGO (A)</t>
         </is>
       </c>
     </row>

</xml_diff>